<commit_message>
1 hot encoding & auc
</commit_message>
<xml_diff>
--- a/csv/AUC_070223.xlsx
+++ b/csv/AUC_070223.xlsx
@@ -270,12 +270,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -290,9 +296,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaallaad" xfId="0" builtinId="0"/>
@@ -576,7 +583,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,7 +678,7 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -720,7 +727,7 @@
       <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="1">
@@ -878,7 +885,7 @@
       <c r="D13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -904,7 +911,7 @@
       <c r="E14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G14" s="1">

</xml_diff>